<commit_message>
update to results table
</commit_message>
<xml_diff>
--- a/simulation_results.xlsx
+++ b/simulation_results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23812"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="13180" yWindow="780" windowWidth="26940" windowHeight="13920" tabRatio="500"/>
+    <workbookView xWindow="26040" yWindow="1480" windowWidth="26940" windowHeight="13920" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="simulation_results.csv" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="29">
   <si>
     <t>basecompdata.18</t>
   </si>
@@ -186,8 +186,54 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -209,13 +255,59 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="53">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -545,10 +637,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L27"/>
+  <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1306,6 +1398,292 @@
         <v>21</v>
       </c>
     </row>
+    <row r="30" spans="1:12">
+      <c r="A30" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="B31" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="A32" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32" s="8">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>0.02</v>
+      </c>
+      <c r="E32">
+        <v>0.03</v>
+      </c>
+      <c r="F32" s="8">
+        <v>1</v>
+      </c>
+      <c r="G32" s="8">
+        <v>1</v>
+      </c>
+      <c r="H32" s="8">
+        <v>0.94</v>
+      </c>
+      <c r="I32" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B33">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C33">
+        <v>0.12</v>
+      </c>
+      <c r="D33">
+        <v>0.11</v>
+      </c>
+      <c r="E33">
+        <v>0.12</v>
+      </c>
+      <c r="F33">
+        <v>0.17</v>
+      </c>
+      <c r="G33">
+        <v>0.13</v>
+      </c>
+      <c r="H33" s="8">
+        <v>1</v>
+      </c>
+      <c r="I33" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34">
+        <v>0.01</v>
+      </c>
+      <c r="C34" s="8">
+        <v>1</v>
+      </c>
+      <c r="D34">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="E34">
+        <v>0.05</v>
+      </c>
+      <c r="F34" s="8">
+        <v>1</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34" s="8">
+        <v>0.95</v>
+      </c>
+      <c r="I34" s="2">
+        <v>0.60762329999999998</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35">
+        <v>0.01</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>0.01</v>
+      </c>
+      <c r="E35">
+        <v>0.01</v>
+      </c>
+      <c r="F35">
+        <v>0.17</v>
+      </c>
+      <c r="G35">
+        <v>0.01</v>
+      </c>
+      <c r="H35">
+        <v>0.06</v>
+      </c>
+      <c r="I35">
+        <v>0.48654710000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>0.03</v>
+      </c>
+      <c r="E36">
+        <v>0.01</v>
+      </c>
+      <c r="F36">
+        <v>0.1</v>
+      </c>
+      <c r="G36">
+        <v>0.01</v>
+      </c>
+      <c r="H36">
+        <v>0.02</v>
+      </c>
+      <c r="I36">
+        <v>8.9686100000000005E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B37">
+        <v>0.01</v>
+      </c>
+      <c r="C37" s="8">
+        <v>1</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37" s="8">
+        <v>1</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+      <c r="H37">
+        <v>0.03</v>
+      </c>
+      <c r="I37" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B38">
+        <v>0</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38" s="8">
+        <v>1</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B39" s="4">
+        <v>5.6815568810851298</v>
+      </c>
+      <c r="C39">
+        <v>5.6910530890221001</v>
+      </c>
+      <c r="D39" s="4">
+        <v>2.9680058837344698</v>
+      </c>
+      <c r="E39" s="4">
+        <v>1.9717815990820799</v>
+      </c>
+      <c r="F39" s="5">
+        <v>14.1053350763073</v>
+      </c>
+      <c r="G39">
+        <v>0.91893766099940899</v>
+      </c>
+      <c r="H39" s="5">
+        <v>46.780758118961302</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B40" s="4">
+        <v>2.0169080981597536</v>
+      </c>
+      <c r="C40" s="9">
+        <v>10.494301464257399</v>
+      </c>
+      <c r="D40" s="4">
+        <v>2.198902871996737</v>
+      </c>
+      <c r="E40" s="4">
+        <v>1.79980371207406</v>
+      </c>
+      <c r="F40" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G40" s="9">
+        <v>1.6136291314399249</v>
+      </c>
+      <c r="H40" s="9">
+        <v>30.627815407750695</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
New genomes added. Old unnecessary genomes removed.
</commit_message>
<xml_diff>
--- a/simulation_results.xlsx
+++ b/simulation_results.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23812"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27100" windowHeight="14480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="simulation_results.csv" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="112">
   <si>
     <t>basecompdata.18</t>
   </si>
@@ -112,12 +112,258 @@
   </si>
   <si>
     <t>Birds proporton of failure</t>
+  </si>
+  <si>
+    <t>Mammals Results</t>
+  </si>
+  <si>
+    <t>Tree shrew sister</t>
+  </si>
+  <si>
+    <t>Primates</t>
+  </si>
+  <si>
+    <t>Rodents</t>
+  </si>
+  <si>
+    <t>Cetartiodactyla sister</t>
+  </si>
+  <si>
+    <t>Chiroptera</t>
+  </si>
+  <si>
+    <t>All loci STAR</t>
+  </si>
+  <si>
+    <t>All loci ASTRAL</t>
+  </si>
+  <si>
+    <t>Homomplasy pass STAR</t>
+  </si>
+  <si>
+    <t>Homoplasy fail STAR</t>
+  </si>
+  <si>
+    <t>Homoplasy fail ASTRAL</t>
+  </si>
+  <si>
+    <t>Homomplasy pass ASTRAL</t>
+  </si>
+  <si>
+    <t>Birds Results</t>
+  </si>
+  <si>
+    <t>Strisores</t>
+  </si>
+  <si>
+    <t>Columbaves</t>
+  </si>
+  <si>
+    <t>Gruiformes</t>
+  </si>
+  <si>
+    <t>Aequorlithornithes</t>
+  </si>
+  <si>
+    <t>Inopinaves</t>
+  </si>
+  <si>
+    <t>Chi-squared pass STAR</t>
+  </si>
+  <si>
+    <t>Chi-squared pass ASTRAL</t>
+  </si>
+  <si>
+    <t>Homoplasy pass STAR</t>
+  </si>
+  <si>
+    <t>Homoplasy pass ASTRAL</t>
+  </si>
+  <si>
+    <t>Chi-squared homoplasy pass STAR</t>
+  </si>
+  <si>
+    <t>Chi-squared homoplasy pass ASTRAL</t>
+  </si>
+  <si>
+    <t>Chi-squared fail STAR</t>
+  </si>
+  <si>
+    <t>Chi-squared fail ASTRAL</t>
+  </si>
+  <si>
+    <t>Inopinaves minus Hoatzin</t>
+  </si>
+  <si>
+    <t>mean empirical branch sup</t>
+  </si>
+  <si>
+    <t>Proportion of failed analyses (mean P-values)</t>
+  </si>
+  <si>
+    <t>0 (0.46)</t>
+  </si>
+  <si>
+    <t>0.07 (0.71)</t>
+  </si>
+  <si>
+    <t>0.01 (0.76)</t>
+  </si>
+  <si>
+    <t>0.01 (0.69)</t>
+  </si>
+  <si>
+    <t>0 (43)</t>
+  </si>
+  <si>
+    <t>0.01 (0.39)</t>
+  </si>
+  <si>
+    <t>0 (0.45)</t>
+  </si>
+  <si>
+    <t>1 (1)</t>
+  </si>
+  <si>
+    <t>0.12 (0.62)</t>
+  </si>
+  <si>
+    <t>1 (0)</t>
+  </si>
+  <si>
+    <t>0 (0.53)</t>
+  </si>
+  <si>
+    <t>0 (0.4)</t>
+  </si>
+  <si>
+    <t>0 (0.49)</t>
+  </si>
+  <si>
+    <t>0.02 (0.32)</t>
+  </si>
+  <si>
+    <t>0.11 (0.78)</t>
+  </si>
+  <si>
+    <t>0.14 (0.57)</t>
+  </si>
+  <si>
+    <t>0.01 (0.59)</t>
+  </si>
+  <si>
+    <t>0.03 (0.49)</t>
+  </si>
+  <si>
+    <t>0 (0.32)</t>
+  </si>
+  <si>
+    <t>0.03 (0.33)</t>
+  </si>
+  <si>
+    <t>0.12 (0.76)</t>
+  </si>
+  <si>
+    <t>0.05 (0.38)</t>
+  </si>
+  <si>
+    <t>0.01 (0.58)</t>
+  </si>
+  <si>
+    <t>0.01 (0.51)</t>
+  </si>
+  <si>
+    <t>0.17 (0.19)</t>
+  </si>
+  <si>
+    <t>0.17 (0.21)</t>
+  </si>
+  <si>
+    <t>0.1 (0.31)</t>
+  </si>
+  <si>
+    <t>0.13 (0.51)</t>
+  </si>
+  <si>
+    <t>0 (0.57)</t>
+  </si>
+  <si>
+    <t>0.01 (0.34)</t>
+  </si>
+  <si>
+    <t>0.01 (0.7)</t>
+  </si>
+  <si>
+    <t>0 (0.6)</t>
+  </si>
+  <si>
+    <t>0 (0.41)</t>
+  </si>
+  <si>
+    <t>0.94 (0.002)</t>
+  </si>
+  <si>
+    <t>0.95 (0.99)</t>
+  </si>
+  <si>
+    <t>0.06 (0.5)</t>
+  </si>
+  <si>
+    <t>0.02 (0.51)</t>
+  </si>
+  <si>
+    <t>0.03 (0.8)</t>
+  </si>
+  <si>
+    <t>0 (5)</t>
+  </si>
+  <si>
+    <t>1 (0.025)</t>
+  </si>
+  <si>
+    <t>0.61 (0.47)</t>
+  </si>
+  <si>
+    <t>0.49 (0.94)</t>
+  </si>
+  <si>
+    <t>0.09 (0.543)</t>
+  </si>
+  <si>
+    <t>0 (0.43)</t>
+  </si>
+  <si>
+    <t>0.99 (0.99)</t>
+  </si>
+  <si>
+    <t>0.80 (0.89)</t>
+  </si>
+  <si>
+    <t>0.85 (0.52)</t>
+  </si>
+  <si>
+    <t>0.56 (0.2)</t>
+  </si>
+  <si>
+    <t>0.93 (0.01)</t>
+  </si>
+  <si>
+    <t>0.98 (0.025)</t>
+  </si>
+  <si>
+    <t>0 (0.48)</t>
+  </si>
+  <si>
+    <t>Carnivora-Prissodactyla</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="169" formatCode="0.000"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -183,7 +429,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -191,8 +437,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="55">
+  <cellStyleXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -248,13 +503,46 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -262,62 +550,108 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="55">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+  <cellStyles count="89">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="88" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -647,20 +981,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M40"/>
+  <dimension ref="A1:M69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="K36" sqref="K36"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" customWidth="1"/>
+    <col min="1" max="1" width="23.33203125" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" customWidth="1"/>
+    <col min="3" max="3" width="20.83203125" customWidth="1"/>
     <col min="4" max="4" width="18.6640625" customWidth="1"/>
     <col min="5" max="5" width="18.33203125" customWidth="1"/>
     <col min="6" max="6" width="18.5" customWidth="1"/>
+    <col min="7" max="7" width="22.1640625" customWidth="1"/>
     <col min="8" max="9" width="19" customWidth="1"/>
     <col min="10" max="10" width="21.83203125" customWidth="1"/>
     <col min="11" max="11" width="18" customWidth="1"/>
@@ -714,40 +1049,40 @@
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="17">
         <v>2.5048828207373899E-3</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="18">
         <v>0.31080960775954602</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="18">
         <v>0.35366468781502097</v>
       </c>
-      <c r="E3" s="8">
-        <v>1</v>
-      </c>
-      <c r="F3" s="4">
+      <c r="E3" s="17">
+        <v>1</v>
+      </c>
+      <c r="F3" s="19">
         <v>0.458819890934133</v>
       </c>
-      <c r="G3" s="8">
-        <v>1</v>
-      </c>
-      <c r="H3" s="4">
+      <c r="G3" s="17">
+        <v>1</v>
+      </c>
+      <c r="H3" s="19">
         <v>0.51117914239042905</v>
       </c>
-      <c r="I3" s="8">
-        <v>0</v>
-      </c>
-      <c r="J3" s="4">
+      <c r="I3" s="17">
+        <v>0</v>
+      </c>
+      <c r="J3" s="19">
         <v>0.31938981230352398</v>
       </c>
-      <c r="K3" s="4">
+      <c r="K3" s="19">
         <v>0.33011001344375102</v>
       </c>
-      <c r="L3" s="8">
+      <c r="L3" s="11">
         <v>2.4618830000000001E-2</v>
       </c>
-      <c r="M3" s="8">
+      <c r="M3" s="11">
         <v>0.99341614906832298</v>
       </c>
     </row>
@@ -755,40 +1090,40 @@
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="8">
-        <v>1</v>
-      </c>
-      <c r="C4">
+      <c r="B4" s="17">
+        <v>1</v>
+      </c>
+      <c r="C4" s="18">
         <v>0.86048487748687896</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="18">
         <v>0.15248179237145901</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="18">
         <v>0.19419758129884199</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="19">
         <v>0.71083525906814504</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="18">
         <v>0.62241785308200503</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="19">
         <v>0.41877279019852598</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="18">
         <v>0.506863250291681</v>
       </c>
-      <c r="J4" s="4">
+      <c r="J4" s="19">
         <v>0.78336891626379201</v>
       </c>
-      <c r="K4" s="4">
+      <c r="K4" s="19">
         <v>0.75611997803562203</v>
       </c>
-      <c r="L4" s="8">
-        <v>1</v>
-      </c>
-      <c r="M4">
+      <c r="L4" s="11">
+        <v>1</v>
+      </c>
+      <c r="M4" s="12">
         <v>0.89751552795031098</v>
       </c>
     </row>
@@ -796,40 +1131,40 @@
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="17">
         <v>0.99958976743713002</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="18">
         <v>0.58865351010848699</v>
       </c>
-      <c r="D5" s="8">
-        <v>1</v>
-      </c>
-      <c r="E5" s="8">
-        <v>0</v>
-      </c>
-      <c r="F5" s="4">
+      <c r="D5" s="17">
+        <v>1</v>
+      </c>
+      <c r="E5" s="17">
+        <v>0</v>
+      </c>
+      <c r="F5" s="19">
         <v>0.75555643663849503</v>
       </c>
-      <c r="G5" s="8">
-        <v>0</v>
-      </c>
-      <c r="H5" s="4">
+      <c r="G5" s="17">
+        <v>0</v>
+      </c>
+      <c r="H5" s="19">
         <v>0.25465695425162999</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="18">
         <v>0.57497827645127297</v>
       </c>
-      <c r="J5" s="4">
+      <c r="J5" s="19">
         <v>0.57493191520846199</v>
       </c>
-      <c r="K5" s="4">
+      <c r="K5" s="19">
         <v>0.37728321784484498</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="12">
         <v>0.47067265000000003</v>
       </c>
-      <c r="M5">
+      <c r="M5" s="12">
         <v>0.52422360248447197</v>
       </c>
     </row>
@@ -837,40 +1172,40 @@
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="18">
         <v>0.49768441020865301</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="18">
         <v>0.77937296166000303</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="18">
         <v>0.78323365350460095</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="18">
         <v>0.21385484100576199</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="19">
         <v>0.68678711009173798</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="18">
         <v>0.52617474319083102</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="19">
         <v>0.62484421076388796</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="18">
         <v>0.344441999679578</v>
       </c>
-      <c r="J6" s="4">
+      <c r="J6" s="19">
         <v>0.58683693943181403</v>
       </c>
-      <c r="K6" s="4">
+      <c r="K6" s="19">
         <v>0.57628477297925496</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="12">
         <v>9.3699550000000006E-2</v>
       </c>
-      <c r="M6">
+      <c r="M6" s="12">
         <v>0.20360248447205001</v>
       </c>
     </row>
@@ -878,40 +1213,40 @@
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="18">
         <v>0.51234228806250903</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="18">
         <v>0.30346493417574</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="18">
         <v>0.40816162788215699</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="18">
         <v>0.30637652947598398</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="19">
         <v>0.42735325678303299</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="18">
         <v>0.400920647293942</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="19">
         <v>0.54869268765470403</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="18">
         <v>0.697726114296783</v>
       </c>
-      <c r="J7" s="4">
+      <c r="J7" s="19">
         <v>0.49140940361569202</v>
       </c>
-      <c r="K7" s="4">
+      <c r="K7" s="19">
         <v>0.51237199751491802</v>
       </c>
-      <c r="L7">
+      <c r="L7" s="12">
         <v>0.542713</v>
       </c>
-      <c r="M7" s="8">
+      <c r="M7" s="11">
         <v>9.8136645962732891E-3</v>
       </c>
     </row>
@@ -919,40 +1254,40 @@
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="18">
         <v>0.79919787151559796</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="17">
         <v>0.94905541420478101</v>
       </c>
-      <c r="D8" s="8">
-        <v>0</v>
-      </c>
-      <c r="E8" s="8">
-        <v>0</v>
-      </c>
-      <c r="F8" s="4">
+      <c r="D8" s="17">
+        <v>0</v>
+      </c>
+      <c r="E8" s="17">
+        <v>0</v>
+      </c>
+      <c r="F8" s="19">
         <v>0.39428668183923699</v>
       </c>
-      <c r="G8" s="8">
-        <v>1</v>
-      </c>
-      <c r="H8" s="4">
+      <c r="G8" s="17">
+        <v>1</v>
+      </c>
+      <c r="H8" s="19">
         <v>0.89512872249442099</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="18">
         <v>0.60323618239535304</v>
       </c>
-      <c r="J8" s="4">
+      <c r="J8" s="19">
         <v>0.45291412190901698</v>
       </c>
-      <c r="K8" s="4">
+      <c r="K8" s="19">
         <v>0.53415252423537596</v>
       </c>
-      <c r="L8" s="8">
-        <v>0</v>
-      </c>
-      <c r="M8" s="8">
+      <c r="L8" s="11">
+        <v>0</v>
+      </c>
+      <c r="M8" s="11">
         <v>2.4720496894409898E-2</v>
       </c>
     </row>
@@ -960,40 +1295,40 @@
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="18">
         <v>0.50363321201859501</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="18">
         <v>0.448021484979158</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="18">
         <v>0.79507586355269</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="17">
         <v>0.99997787473606903</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="19">
         <v>0.45494635333716898</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="18">
         <v>0.48514702162208401</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H9" s="19">
         <v>0.44090470941423998</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="18">
         <v>0.40506134161371499</v>
       </c>
-      <c r="J9" s="4">
+      <c r="J9" s="19">
         <v>0.323462736295619</v>
       </c>
-      <c r="K9" s="4">
+      <c r="K9" s="19">
         <v>0.44960223959421097</v>
       </c>
-      <c r="L9">
+      <c r="L9" s="12">
         <v>0.42529148</v>
       </c>
-      <c r="M9">
+      <c r="M9" s="12">
         <v>0.48043478260869599</v>
       </c>
     </row>
@@ -1001,112 +1336,116 @@
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="20">
         <v>46.780758118961302</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="20">
         <v>37.517213529791903</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="20">
         <v>7.29343813532713</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="20">
         <v>14.1053350763073</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="19">
         <v>5.6815568810851298</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="18">
         <v>5.6910530890221001</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H10" s="19">
         <v>4.3412383900045697</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="18">
         <v>0.91893766099940899</v>
       </c>
-      <c r="J10" s="4">
+      <c r="J10" s="19">
         <v>2.9680058837344698</v>
       </c>
-      <c r="K10" s="4">
+      <c r="K10" s="19">
         <v>1.9717815990820799</v>
       </c>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
     </row>
     <row r="11" spans="1:13">
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="20">
         <v>0.91883446223252097</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="20">
         <v>2.32861629882261</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="20">
         <v>615.29735631234905</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="20">
         <v>1123.03812426131</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="19">
         <v>6.0507242944792601E-2</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G11" s="20">
         <v>0.31482904392772199</v>
       </c>
-      <c r="H11" s="4">
+      <c r="H11" s="19">
         <v>5.1422560996839499E-2</v>
       </c>
-      <c r="I11" s="5">
+      <c r="I11" s="20">
         <v>0.19363549577279099</v>
       </c>
-      <c r="J11" s="4">
+      <c r="J11" s="19">
         <v>6.59670861599021E-2</v>
       </c>
-      <c r="K11" s="4">
+      <c r="K11" s="19">
         <v>5.3994111362221799E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" s="9" customFormat="1">
-      <c r="A12" s="11" t="s">
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+    </row>
+    <row r="12" spans="1:13" s="8" customFormat="1">
+      <c r="A12" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="9">
+      <c r="B12" s="15">
         <v>30.627815407750695</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="11">
         <v>77.620543294087</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="13">
         <v>2.0169080981597536</v>
       </c>
-      <c r="G12" s="9">
+      <c r="G12" s="15">
         <v>10.494301464257399</v>
       </c>
-      <c r="H12" s="4">
+      <c r="H12" s="13">
         <v>0.85704268328065836</v>
       </c>
-      <c r="I12" s="9">
+      <c r="I12" s="15">
         <v>1.6136291314399249</v>
       </c>
-      <c r="J12" s="4">
+      <c r="J12" s="13">
         <v>2.198902871996737</v>
       </c>
-      <c r="K12" s="4">
+      <c r="K12" s="13">
         <v>1.79980371207406</v>
       </c>
     </row>
-    <row r="13" spans="1:13" s="9" customFormat="1">
-      <c r="A13" s="11"/>
-    </row>
-    <row r="14" spans="1:13" s="9" customFormat="1">
-      <c r="A14" s="11" t="s">
+    <row r="13" spans="1:13" s="8" customFormat="1">
+      <c r="A13" s="10"/>
+    </row>
+    <row r="14" spans="1:13" s="8" customFormat="1">
+      <c r="A14" s="10" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1152,7 +1491,7 @@
       <c r="A16" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="8">
+      <c r="B16" s="7">
         <v>0.94</v>
       </c>
       <c r="C16">
@@ -1161,19 +1500,19 @@
       <c r="D16" s="2">
         <v>0.85</v>
       </c>
-      <c r="E16" s="8">
+      <c r="E16" s="7">
         <v>1</v>
       </c>
       <c r="F16">
         <v>0</v>
       </c>
-      <c r="G16" s="8">
+      <c r="G16" s="7">
         <v>1</v>
       </c>
       <c r="H16">
         <v>0</v>
       </c>
-      <c r="I16" s="8">
+      <c r="I16" s="7">
         <v>1</v>
       </c>
       <c r="J16">
@@ -1182,10 +1521,10 @@
       <c r="K16">
         <v>0.03</v>
       </c>
-      <c r="L16" s="8">
-        <v>1</v>
-      </c>
-      <c r="M16" s="8">
+      <c r="L16" s="7">
+        <v>1</v>
+      </c>
+      <c r="M16" s="7">
         <v>0.99</v>
       </c>
     </row>
@@ -1193,7 +1532,7 @@
       <c r="A17" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="8">
+      <c r="B17" s="7">
         <v>1</v>
       </c>
       <c r="C17">
@@ -1223,10 +1562,10 @@
       <c r="K17">
         <v>0.12</v>
       </c>
-      <c r="L17" s="8">
-        <v>1</v>
-      </c>
-      <c r="M17" s="2">
+      <c r="L17" s="7">
+        <v>1</v>
+      </c>
+      <c r="M17" s="16">
         <v>0.80124220000000002</v>
       </c>
     </row>
@@ -1234,22 +1573,22 @@
       <c r="A18" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="8">
+      <c r="B18" s="7">
         <v>0.95</v>
       </c>
       <c r="C18">
         <v>0.06</v>
       </c>
-      <c r="D18" s="8">
-        <v>1</v>
-      </c>
-      <c r="E18" s="8">
+      <c r="D18" s="7">
+        <v>1</v>
+      </c>
+      <c r="E18" s="7">
         <v>1</v>
       </c>
       <c r="F18">
         <v>0.01</v>
       </c>
-      <c r="G18" s="8">
+      <c r="G18" s="7">
         <v>1</v>
       </c>
       <c r="H18">
@@ -1264,10 +1603,10 @@
       <c r="K18">
         <v>0.05</v>
       </c>
-      <c r="L18" s="2">
+      <c r="L18" s="16">
         <v>0.60762329999999998</v>
       </c>
-      <c r="M18" s="2">
+      <c r="M18" s="16">
         <v>0.85093169999999996</v>
       </c>
     </row>
@@ -1305,10 +1644,10 @@
       <c r="K19">
         <v>0.01</v>
       </c>
-      <c r="L19">
+      <c r="L19" s="12">
         <v>0.48654710000000001</v>
       </c>
-      <c r="M19" s="2">
+      <c r="M19" s="16">
         <v>0.55900620000000001</v>
       </c>
     </row>
@@ -1346,10 +1685,10 @@
       <c r="K20">
         <v>0.01</v>
       </c>
-      <c r="L20">
+      <c r="L20" s="12">
         <v>8.9686100000000005E-2</v>
       </c>
-      <c r="M20" s="2">
+      <c r="M20" s="16">
         <v>0.93167699999999998</v>
       </c>
     </row>
@@ -1363,16 +1702,16 @@
       <c r="C21">
         <v>0.37</v>
       </c>
-      <c r="D21" s="8">
-        <v>1</v>
-      </c>
-      <c r="E21" s="8">
+      <c r="D21" s="7">
+        <v>1</v>
+      </c>
+      <c r="E21" s="7">
         <v>1</v>
       </c>
       <c r="F21">
         <v>0.01</v>
       </c>
-      <c r="G21" s="8">
+      <c r="G21" s="7">
         <v>1</v>
       </c>
       <c r="H21">
@@ -1387,10 +1726,10 @@
       <c r="K21">
         <v>0</v>
       </c>
-      <c r="L21" s="8">
-        <v>1</v>
-      </c>
-      <c r="M21" s="8">
+      <c r="L21" s="7">
+        <v>1</v>
+      </c>
+      <c r="M21" s="11">
         <v>0.97515529999999995</v>
       </c>
     </row>
@@ -1407,7 +1746,7 @@
       <c r="D22">
         <v>0.8</v>
       </c>
-      <c r="E22" s="8">
+      <c r="E22" s="7">
         <v>1</v>
       </c>
       <c r="F22">
@@ -1435,335 +1774,821 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:13">
-      <c r="C24" s="9"/>
-      <c r="D24" s="10" t="s">
+    <row r="23" spans="1:13">
+      <c r="A23" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" s="12">
+        <v>0.91594336055665004</v>
+      </c>
+      <c r="C23" s="12">
+        <v>0.92584157211590501</v>
+      </c>
+      <c r="D23" s="12">
+        <v>0.87991494514972901</v>
+      </c>
+      <c r="E23" s="12">
+        <v>0.820837061576</v>
+      </c>
+      <c r="F23" s="12">
+        <v>0.94172747265493595</v>
+      </c>
+      <c r="G23" s="12">
+        <v>0.97472849286191399</v>
+      </c>
+      <c r="H23" s="12">
+        <v>0.92867829313545602</v>
+      </c>
+      <c r="I23" s="12">
+        <v>0.915194570136868</v>
+      </c>
+      <c r="J23" s="12">
+        <v>0.95085616921175498</v>
+      </c>
+      <c r="K23" s="12">
+        <v>0.95062371425560899</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="C25" s="8"/>
+      <c r="D25" s="9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:13">
-      <c r="D25" s="6" t="s">
+    <row r="26" spans="1:13">
+      <c r="D26" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:13">
-      <c r="D26" s="7" t="s">
+    <row r="27" spans="1:13">
+      <c r="D27" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:13">
-      <c r="D27" s="3" t="s">
+    <row r="28" spans="1:13">
+      <c r="D28" s="3" t="s">
         <v>21</v>
       </c>
     </row>
+    <row r="29" spans="1:13">
+      <c r="A29" s="21"/>
+      <c r="B29" s="21"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="21"/>
+      <c r="I29" s="21"/>
+      <c r="J29" s="21"/>
+      <c r="K29" s="21"/>
+    </row>
     <row r="30" spans="1:13">
-      <c r="A30" s="11" t="s">
-        <v>23</v>
-      </c>
+      <c r="A30" s="22"/>
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="22"/>
+      <c r="H30" s="22"/>
+      <c r="I30" s="22"/>
+      <c r="J30" s="22"/>
+      <c r="K30" s="22"/>
     </row>
     <row r="31" spans="1:13">
-      <c r="B31" s="1" t="s">
+      <c r="A31" s="22"/>
+      <c r="B31" s="22"/>
+      <c r="C31" s="22"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="22"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="22"/>
+      <c r="H31" s="22"/>
+      <c r="I31" s="22"/>
+      <c r="J31" s="22"/>
+      <c r="K31" s="22"/>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" s="10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="B34" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C34" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D34" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E34" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="F34" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G31" s="1" t="s">
+      <c r="G34" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H31" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I31" s="1" t="s">
+      <c r="H34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I34" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="J31" s="1" t="s">
+      <c r="J34" s="1" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13">
-      <c r="A32" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B32">
-        <v>0</v>
-      </c>
-      <c r="C32" s="8">
-        <v>1</v>
-      </c>
-      <c r="D32">
-        <v>0.02</v>
-      </c>
-      <c r="E32">
-        <v>0.03</v>
-      </c>
-      <c r="F32" s="8">
-        <v>1</v>
-      </c>
-      <c r="G32" s="8">
-        <v>1</v>
-      </c>
-      <c r="H32" s="8">
-        <v>0.94</v>
-      </c>
-      <c r="I32" s="8">
-        <v>1</v>
-      </c>
-      <c r="J32" s="8">
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10">
-      <c r="A33" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B33">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C33">
-        <v>0.12</v>
-      </c>
-      <c r="D33">
-        <v>0.11</v>
-      </c>
-      <c r="E33">
-        <v>0.12</v>
-      </c>
-      <c r="F33">
-        <v>0.17</v>
-      </c>
-      <c r="G33">
-        <v>0.13</v>
-      </c>
-      <c r="H33" s="8">
-        <v>1</v>
-      </c>
-      <c r="I33" s="8">
-        <v>1</v>
-      </c>
-      <c r="J33" s="2">
-        <v>0.80124220000000002</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10">
-      <c r="A34" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B34">
-        <v>0.01</v>
-      </c>
-      <c r="C34" s="8">
-        <v>1</v>
-      </c>
-      <c r="D34">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="E34">
-        <v>0.05</v>
-      </c>
-      <c r="F34" s="8">
-        <v>1</v>
-      </c>
-      <c r="G34">
-        <v>0</v>
-      </c>
-      <c r="H34" s="8">
-        <v>0.95</v>
-      </c>
-      <c r="I34" s="2">
-        <v>0.60762329999999998</v>
-      </c>
-      <c r="J34" s="2">
-        <v>0.85093169999999996</v>
       </c>
     </row>
     <row r="35" spans="1:10">
       <c r="A35" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B35">
-        <v>0.01</v>
-      </c>
-      <c r="C35">
-        <v>0</v>
-      </c>
-      <c r="D35">
-        <v>0.01</v>
-      </c>
-      <c r="E35">
-        <v>0.01</v>
-      </c>
-      <c r="F35">
-        <v>0.17</v>
-      </c>
-      <c r="G35">
-        <v>0.01</v>
-      </c>
-      <c r="H35">
-        <v>0.06</v>
-      </c>
-      <c r="I35">
-        <v>0.48654710000000001</v>
-      </c>
-      <c r="J35" s="2">
-        <v>0.55900620000000001</v>
+        <v>10</v>
+      </c>
+      <c r="B35" t="s">
+        <v>60</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D35" t="s">
+        <v>73</v>
+      </c>
+      <c r="E35" t="s">
+        <v>79</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="G35" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H35" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="I35" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="J35" s="7" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B36">
-        <v>0</v>
-      </c>
-      <c r="C36">
-        <v>0</v>
-      </c>
-      <c r="D36">
-        <v>0.03</v>
-      </c>
-      <c r="E36">
-        <v>0.01</v>
-      </c>
-      <c r="F36">
-        <v>0.1</v>
-      </c>
-      <c r="G36">
-        <v>0.01</v>
-      </c>
-      <c r="H36">
-        <v>0.02</v>
-      </c>
-      <c r="I36">
-        <v>8.9686100000000005E-2</v>
-      </c>
-      <c r="J36" s="2">
-        <v>0.93167699999999998</v>
+        <v>11</v>
+      </c>
+      <c r="B36" t="s">
+        <v>61</v>
+      </c>
+      <c r="C36" t="s">
+        <v>68</v>
+      </c>
+      <c r="D36" t="s">
+        <v>74</v>
+      </c>
+      <c r="E36" t="s">
+        <v>80</v>
+      </c>
+      <c r="F36" t="s">
+        <v>84</v>
+      </c>
+      <c r="G36" t="s">
+        <v>87</v>
+      </c>
+      <c r="H36" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="I36" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="J36" s="16" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="37" spans="1:10">
       <c r="A37" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B37">
-        <v>0.01</v>
-      </c>
-      <c r="C37" s="8">
-        <v>1</v>
-      </c>
-      <c r="D37">
-        <v>0</v>
-      </c>
-      <c r="E37">
-        <v>0</v>
-      </c>
-      <c r="F37" s="8">
-        <v>1</v>
-      </c>
-      <c r="G37">
-        <v>0</v>
-      </c>
-      <c r="H37">
-        <v>0.03</v>
-      </c>
-      <c r="I37" s="8">
-        <v>1</v>
-      </c>
-      <c r="J37" s="8">
-        <v>0.97515529999999995</v>
+        <v>12</v>
+      </c>
+      <c r="B37" t="s">
+        <v>62</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D37" t="s">
+        <v>75</v>
+      </c>
+      <c r="E37" t="s">
+        <v>81</v>
+      </c>
+      <c r="F37" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="G37" t="s">
+        <v>88</v>
+      </c>
+      <c r="H37" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="I37" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="J37" s="16" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="38" spans="1:10">
       <c r="A38" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B38">
-        <v>0</v>
-      </c>
-      <c r="C38">
-        <v>0</v>
-      </c>
-      <c r="D38">
-        <v>0</v>
-      </c>
-      <c r="E38">
-        <v>0</v>
-      </c>
-      <c r="F38" s="8">
-        <v>1</v>
-      </c>
-      <c r="G38">
-        <v>0</v>
-      </c>
-      <c r="H38">
-        <v>0</v>
-      </c>
-      <c r="I38">
-        <v>0</v>
-      </c>
-      <c r="J38">
-        <v>0</v>
+        <v>13</v>
+      </c>
+      <c r="B38" t="s">
+        <v>63</v>
+      </c>
+      <c r="C38" t="s">
+        <v>70</v>
+      </c>
+      <c r="D38" t="s">
+        <v>76</v>
+      </c>
+      <c r="E38" t="s">
+        <v>82</v>
+      </c>
+      <c r="F38" t="s">
+        <v>85</v>
+      </c>
+      <c r="G38" t="s">
+        <v>89</v>
+      </c>
+      <c r="H38" t="s">
+        <v>95</v>
+      </c>
+      <c r="I38" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="J38" s="16" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="39" spans="1:10">
       <c r="A39" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B39" t="s">
+        <v>64</v>
+      </c>
+      <c r="C39" t="s">
+        <v>71</v>
+      </c>
+      <c r="D39" t="s">
+        <v>77</v>
+      </c>
+      <c r="E39" t="s">
+        <v>83</v>
+      </c>
+      <c r="F39" t="s">
+        <v>86</v>
+      </c>
+      <c r="G39" t="s">
+        <v>90</v>
+      </c>
+      <c r="H39" t="s">
+        <v>96</v>
+      </c>
+      <c r="I39" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="J39" s="16" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B40" t="s">
+        <v>65</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D40" t="s">
+        <v>66</v>
+      </c>
+      <c r="E40" t="s">
+        <v>70</v>
+      </c>
+      <c r="F40" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="G40" t="s">
+        <v>91</v>
+      </c>
+      <c r="H40" t="s">
+        <v>97</v>
+      </c>
+      <c r="I40" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="J40" s="11" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="A41" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B41" t="s">
+        <v>66</v>
+      </c>
+      <c r="C41" t="s">
+        <v>72</v>
+      </c>
+      <c r="D41" t="s">
+        <v>78</v>
+      </c>
+      <c r="E41" t="s">
+        <v>66</v>
+      </c>
+      <c r="F41" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="G41" t="s">
+        <v>92</v>
+      </c>
+      <c r="H41" t="s">
+        <v>98</v>
+      </c>
+      <c r="I41" t="s">
+        <v>103</v>
+      </c>
+      <c r="J41" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="A42" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B42" s="14">
+        <v>0.94172747265493595</v>
+      </c>
+      <c r="C42" s="12">
+        <v>0.97472849286191399</v>
+      </c>
+      <c r="D42" s="12">
+        <v>0.95085616921175498</v>
+      </c>
+      <c r="E42" s="12">
+        <v>0.95062371425560899</v>
+      </c>
+      <c r="F42" s="14">
+        <v>0.820837061576</v>
+      </c>
+      <c r="G42" s="14">
+        <v>0.915194570136868</v>
+      </c>
+      <c r="H42" s="14">
+        <v>0.91594336055665004</v>
+      </c>
+      <c r="I42" s="14">
+        <v>0.85429940000000004</v>
+      </c>
+      <c r="J42" s="14">
+        <v>0.77446700000000002</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
+      <c r="A43" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B39" s="4">
+      <c r="B43" s="15">
         <v>5.6815568810851298</v>
       </c>
-      <c r="C39">
+      <c r="C43" s="12">
         <v>5.6910530890221001</v>
       </c>
-      <c r="D39" s="4">
+      <c r="D43" s="15">
         <v>2.9680058837344698</v>
       </c>
-      <c r="E39" s="4">
+      <c r="E43" s="15">
         <v>1.9717815990820799</v>
       </c>
-      <c r="F39" s="5">
+      <c r="F43" s="14">
         <v>14.1053350763073</v>
       </c>
-      <c r="G39">
+      <c r="G43" s="12">
         <v>0.91893766099940899</v>
       </c>
-      <c r="H39" s="5">
+      <c r="H43" s="14">
         <v>46.780758118961302</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
-      <c r="A40" s="11" t="s">
+    <row r="44" spans="1:10">
+      <c r="A44" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B40" s="4">
+      <c r="B44" s="15">
         <v>2.0169080981597536</v>
       </c>
-      <c r="C40" s="9">
+      <c r="C44" s="14">
         <v>10.494301464257399</v>
       </c>
-      <c r="D40" s="4">
+      <c r="D44" s="15">
         <v>2.198902871996737</v>
       </c>
-      <c r="E40" s="4">
+      <c r="E44" s="15">
         <v>1.79980371207406</v>
       </c>
-      <c r="F40" s="8" t="s">
+      <c r="F44" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G40" s="9">
+      <c r="G44" s="15">
         <v>1.6136291314399249</v>
       </c>
-      <c r="H40" s="9">
+      <c r="H44" s="14">
         <v>30.627815407750695</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
+      <c r="A47" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10">
+      <c r="B48" t="s">
+        <v>32</v>
+      </c>
+      <c r="C48" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49" t="s">
+        <v>37</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50" t="s">
+        <v>39</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51" t="s">
+        <v>40</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52" t="s">
+        <v>38</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53" t="s">
+        <v>42</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="A54" t="s">
+        <v>41</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="A56" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
+      <c r="B57" t="s">
+        <v>44</v>
+      </c>
+      <c r="C57" t="s">
+        <v>45</v>
+      </c>
+      <c r="D57" t="s">
+        <v>46</v>
+      </c>
+      <c r="E57" t="s">
+        <v>47</v>
+      </c>
+      <c r="F57" t="s">
+        <v>48</v>
+      </c>
+      <c r="G57" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
+      <c r="A58" t="s">
+        <v>37</v>
+      </c>
+      <c r="B58" s="2">
+        <v>1</v>
+      </c>
+      <c r="C58" s="4">
+        <v>0</v>
+      </c>
+      <c r="D58" s="2">
+        <v>1</v>
+      </c>
+      <c r="E58" s="2">
+        <v>1</v>
+      </c>
+      <c r="F58" s="4">
+        <v>0</v>
+      </c>
+      <c r="G58" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
+      <c r="A59" t="s">
+        <v>49</v>
+      </c>
+      <c r="B59" s="2">
+        <v>1</v>
+      </c>
+      <c r="C59" s="4">
+        <v>0</v>
+      </c>
+      <c r="D59" s="2">
+        <v>1</v>
+      </c>
+      <c r="E59" s="2">
+        <v>1</v>
+      </c>
+      <c r="F59" s="4">
+        <v>0</v>
+      </c>
+      <c r="G59" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
+      <c r="A60" t="s">
+        <v>55</v>
+      </c>
+      <c r="B60" s="2">
+        <v>1</v>
+      </c>
+      <c r="C60" s="4">
+        <v>0</v>
+      </c>
+      <c r="D60" s="2">
+        <v>1</v>
+      </c>
+      <c r="E60" s="2">
+        <v>1</v>
+      </c>
+      <c r="F60" s="4">
+        <v>0</v>
+      </c>
+      <c r="G60" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
+      <c r="A61" t="s">
+        <v>51</v>
+      </c>
+      <c r="B61" s="2">
+        <v>1</v>
+      </c>
+      <c r="C61" s="4">
+        <v>0</v>
+      </c>
+      <c r="D61" s="2">
+        <v>1</v>
+      </c>
+      <c r="E61" s="2">
+        <v>1</v>
+      </c>
+      <c r="F61" s="4">
+        <v>0</v>
+      </c>
+      <c r="G61" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
+      <c r="A62" t="s">
+        <v>40</v>
+      </c>
+      <c r="B62" s="2">
+        <v>1</v>
+      </c>
+      <c r="C62" s="4">
+        <v>0</v>
+      </c>
+      <c r="D62" s="2">
+        <v>1</v>
+      </c>
+      <c r="E62" s="2">
+        <v>1</v>
+      </c>
+      <c r="F62" s="4">
+        <v>0</v>
+      </c>
+      <c r="G62" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
+      <c r="A63" t="s">
+        <v>53</v>
+      </c>
+      <c r="B63" s="4">
+        <v>0</v>
+      </c>
+      <c r="C63" s="4">
+        <v>0</v>
+      </c>
+      <c r="D63" s="2">
+        <v>1</v>
+      </c>
+      <c r="E63" s="2">
+        <v>1</v>
+      </c>
+      <c r="F63" s="4">
+        <v>0</v>
+      </c>
+      <c r="G63" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
+      <c r="A64" t="s">
+        <v>38</v>
+      </c>
+      <c r="B64" s="2">
+        <v>1</v>
+      </c>
+      <c r="C64" s="4">
+        <v>0</v>
+      </c>
+      <c r="D64" s="2">
+        <v>1</v>
+      </c>
+      <c r="E64" s="2">
+        <v>1</v>
+      </c>
+      <c r="F64" s="4">
+        <v>0</v>
+      </c>
+      <c r="G64" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
+      <c r="A65" t="s">
+        <v>50</v>
+      </c>
+      <c r="B65" s="4">
+        <v>0</v>
+      </c>
+      <c r="C65" s="4">
+        <v>0</v>
+      </c>
+      <c r="D65" s="2">
+        <v>1</v>
+      </c>
+      <c r="E65" s="2">
+        <v>1</v>
+      </c>
+      <c r="F65" s="4">
+        <v>0</v>
+      </c>
+      <c r="G65" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
+      <c r="A66" t="s">
+        <v>56</v>
+      </c>
+      <c r="B66" s="2">
+        <v>1</v>
+      </c>
+      <c r="C66" s="4">
+        <v>0</v>
+      </c>
+      <c r="D66" s="2">
+        <v>1</v>
+      </c>
+      <c r="E66" s="2">
+        <v>1</v>
+      </c>
+      <c r="F66" s="4">
+        <v>0</v>
+      </c>
+      <c r="G66" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
+      <c r="A67" t="s">
+        <v>52</v>
+      </c>
+      <c r="B67" s="2">
+        <v>1</v>
+      </c>
+      <c r="C67" s="4">
+        <v>0</v>
+      </c>
+      <c r="D67" s="2">
+        <v>1</v>
+      </c>
+      <c r="E67" s="2">
+        <v>1</v>
+      </c>
+      <c r="F67" s="4">
+        <v>0</v>
+      </c>
+      <c r="G67" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
+      <c r="A68" t="s">
+        <v>41</v>
+      </c>
+      <c r="B68" s="2">
+        <v>1</v>
+      </c>
+      <c r="C68" s="4">
+        <v>0</v>
+      </c>
+      <c r="D68" s="2">
+        <v>1</v>
+      </c>
+      <c r="E68" s="2">
+        <v>1</v>
+      </c>
+      <c r="F68" s="4">
+        <v>0</v>
+      </c>
+      <c r="G68" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
+      <c r="A69" t="s">
+        <v>54</v>
+      </c>
+      <c r="B69" s="4">
+        <v>0</v>
+      </c>
+      <c r="C69" s="4">
+        <v>0</v>
+      </c>
+      <c r="D69" s="2">
+        <v>1</v>
+      </c>
+      <c r="E69" s="2">
+        <v>1</v>
+      </c>
+      <c r="F69" s="4">
+        <v>0</v>
+      </c>
+      <c r="G69" s="4">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>